<commit_message>
Changes to plot stucture for a presentation and general progress on updating some of the scritps.
Plots and figures altered to better suit a presentation format, as well as updates made to allow four polts (one for each gridspacing of 5, 15, 22.5, and 30 degrees). Violin plot should now be functional as well (updated to python 3). Some lines in script commented out to produce the new versions of plots (such as the change to a scatter plot from a bar plot to better show some of the data).  The commented lines can be used to revert to the previous plotting formats.
</commit_message>
<xml_diff>
--- a/JupyterNotebooks/AveragedIntensites/BrassA-HW20.xlsx
+++ b/JupyterNotebooks/AveragedIntensites/BrassA-HW20.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Temp\Documents\GitHub\Texture-Sampling-PhaseMeasurement-BiasErrors\JupyterNotebooks\AveragedIntensites\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28100C6-8C05-42F7-9B7A-D476CEC766DA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-3720" yWindow="2595" windowWidth="7500" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BrassA-HW20.xpc" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -103,8 +109,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,6 +173,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -213,7 +227,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -245,9 +259,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -279,6 +311,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -454,14 +504,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -508,7 +560,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -558,7 +610,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -587,7 +639,7 @@
         <v>1.5</v>
       </c>
       <c r="J3">
-        <v>1.15</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="K3">
         <v>0.84</v>
@@ -602,13 +654,13 @@
         <v>1.095</v>
       </c>
       <c r="O3">
-        <v>0.8925000000000001</v>
+        <v>0.89250000000000007</v>
       </c>
       <c r="P3">
-        <v>0.94375</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+        <v>0.94374999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -658,7 +710,7 @@
         <v>0.96875</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -699,16 +751,16 @@
         <v>1.55</v>
       </c>
       <c r="N5">
-        <v>0.635</v>
+        <v>0.63500000000000001</v>
       </c>
       <c r="O5">
         <v>0.9524999999999999</v>
       </c>
       <c r="P5">
-        <v>0.9562499999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+        <v>0.95624999999999993</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -737,7 +789,7 @@
         <v>1.48</v>
       </c>
       <c r="J6">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="K6">
         <v>0.84</v>
@@ -752,13 +804,13 @@
         <v>1.08</v>
       </c>
       <c r="O6">
-        <v>0.8875</v>
+        <v>0.88749999999999996</v>
       </c>
       <c r="P6">
         <v>0.9325</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -766,49 +818,49 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>1.405753424657534</v>
+        <v>1.4057534246575341</v>
       </c>
       <c r="D7">
-        <v>0.9704109589041096</v>
+        <v>0.97041095890410956</v>
       </c>
       <c r="E7">
-        <v>0.8561643835616438</v>
+        <v>0.85616438356164382</v>
       </c>
       <c r="F7">
-        <v>0.9330136986301369</v>
+        <v>0.93301369863013695</v>
       </c>
       <c r="G7">
-        <v>1.405753424657534</v>
+        <v>1.4057534246575341</v>
       </c>
       <c r="H7">
-        <v>0.9704109589041096</v>
+        <v>0.97041095890410956</v>
       </c>
       <c r="I7">
-        <v>1.021780821917808</v>
+        <v>1.0217808219178079</v>
       </c>
       <c r="J7">
-        <v>0.8382191780821918</v>
+        <v>0.83821917808219182</v>
       </c>
       <c r="K7">
         <v>1.098356164383562</v>
       </c>
       <c r="L7">
-        <v>0.9063013698630137</v>
+        <v>0.90630136986301368</v>
       </c>
       <c r="M7">
         <v>1.405342465753425</v>
       </c>
       <c r="N7">
-        <v>0.9132876712328767</v>
+        <v>0.91328767123287669</v>
       </c>
       <c r="O7">
         <v>1.041335616438356</v>
       </c>
       <c r="P7">
-        <v>1.00375</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
+        <v>1.0037499999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -816,49 +868,49 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D8">
-        <v>0.348421052631579</v>
+        <v>0.34842105263157902</v>
       </c>
       <c r="E8">
         <v>1.384736842105263</v>
       </c>
       <c r="F8">
-        <v>0.8489473684210527</v>
+        <v>0.84894736842105267</v>
       </c>
       <c r="G8">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H8">
-        <v>0.348421052631579</v>
+        <v>0.34842105263157902</v>
       </c>
       <c r="I8">
-        <v>1.283157894736842</v>
+        <v>1.2831578947368421</v>
       </c>
       <c r="J8">
-        <v>0.9694736842105263</v>
+        <v>0.96947368421052627</v>
       </c>
       <c r="K8">
         <v>1.053684210526316</v>
       </c>
       <c r="L8">
-        <v>0.5821052631578948</v>
+        <v>0.58210526315789479</v>
       </c>
       <c r="M8">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="N8">
-        <v>0.8665789473684211</v>
+        <v>0.86657894736842112</v>
       </c>
       <c r="O8">
-        <v>0.9205263157894737</v>
+        <v>0.92052631578947375</v>
       </c>
       <c r="P8">
-        <v>0.9463157894736842</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
+        <v>0.94631578947368422</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -866,28 +918,28 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>1.092105263157895</v>
+        <v>1.0921052631578949</v>
       </c>
       <c r="D9">
-        <v>0.6736842105263158</v>
+        <v>0.67368421052631577</v>
       </c>
       <c r="E9">
-        <v>1.102105263157895</v>
+        <v>1.1021052631578949</v>
       </c>
       <c r="F9">
-        <v>0.9526315789473684</v>
+        <v>0.95263157894736838</v>
       </c>
       <c r="G9">
-        <v>1.092105263157895</v>
+        <v>1.0921052631578949</v>
       </c>
       <c r="H9">
-        <v>0.6736842105263158</v>
+        <v>0.67368421052631577</v>
       </c>
       <c r="I9">
         <v>1.092631578947368</v>
       </c>
       <c r="J9">
-        <v>0.9794736842105263</v>
+        <v>0.97947368421052627</v>
       </c>
       <c r="K9">
         <v>1.044210526315789</v>
@@ -896,19 +948,19 @@
         <v>0.8242105263157895</v>
       </c>
       <c r="M9">
-        <v>1.092105263157895</v>
+        <v>1.0921052631578949</v>
       </c>
       <c r="N9">
-        <v>0.8878947368421053</v>
+        <v>0.88789473684210529</v>
       </c>
       <c r="O9">
-        <v>0.9551315789473684</v>
+        <v>0.95513157894736844</v>
       </c>
       <c r="P9">
-        <v>0.9701315789473683</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
+        <v>0.97013157894736834</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -916,10 +968,10 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>0.6529599999999995</v>
+        <v>0.65295999999999954</v>
       </c>
       <c r="D10">
-        <v>0.5621440000000003</v>
+        <v>0.56214400000000031</v>
       </c>
       <c r="E10">
         <v>1.571404</v>
@@ -928,37 +980,37 @@
         <v>0.8727600000000002</v>
       </c>
       <c r="G10">
-        <v>0.6529599999999995</v>
+        <v>0.65295999999999954</v>
       </c>
       <c r="H10">
-        <v>0.5621440000000003</v>
+        <v>0.56214400000000031</v>
       </c>
       <c r="I10">
-        <v>1.247939999999997</v>
+        <v>1.2479399999999969</v>
       </c>
       <c r="J10">
-        <v>1.141883999999998</v>
+        <v>1.1418839999999979</v>
       </c>
       <c r="K10">
-        <v>0.8743560000000007</v>
+        <v>0.87435600000000069</v>
       </c>
       <c r="L10">
-        <v>0.7628520000000003</v>
+        <v>0.76285200000000031</v>
       </c>
       <c r="M10">
-        <v>0.6529599999999995</v>
+        <v>0.65295999999999954</v>
       </c>
       <c r="N10">
-        <v>1.066774</v>
+        <v>1.0667740000000001</v>
       </c>
       <c r="O10">
-        <v>0.914817</v>
+        <v>0.91481699999999999</v>
       </c>
       <c r="P10">
-        <v>0.9607874999999995</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
+        <v>0.96078749999999946</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -975,7 +1027,7 @@
         <v>1.979862499999999</v>
       </c>
       <c r="F11">
-        <v>0.696262499999999</v>
+        <v>0.69626249999999901</v>
       </c>
       <c r="G11">
         <v>0.68</v>
@@ -987,7 +1039,7 @@
         <v>1.5</v>
       </c>
       <c r="J11">
-        <v>1.15</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="K11">
         <v>0.84</v>
@@ -999,16 +1051,16 @@
         <v>0.68</v>
       </c>
       <c r="N11">
-        <v>1.09493125</v>
+        <v>1.0949312499999999</v>
       </c>
       <c r="O11">
-        <v>0.8915312499999996</v>
+        <v>0.89153124999999955</v>
       </c>
       <c r="P11">
-        <v>0.9432656249999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
+        <v>0.94326562499999977</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1022,10 +1074,10 @@
         <v>0.5401972946944007</v>
       </c>
       <c r="E12">
-        <v>1.560636958208003</v>
+        <v>1.5606369582080031</v>
       </c>
       <c r="F12">
-        <v>0.8248496616447993</v>
+        <v>0.82484966164479934</v>
       </c>
       <c r="G12">
         <v>0.8210743283712032</v>
@@ -1037,28 +1089,28 @@
         <v>1.282742223872001</v>
       </c>
       <c r="J12">
-        <v>1.080514512076795</v>
+        <v>1.0805145120767949</v>
       </c>
       <c r="K12">
-        <v>0.9089590743040022</v>
+        <v>0.90895907430400225</v>
       </c>
       <c r="L12">
-        <v>0.7039447246848015</v>
+        <v>0.70394472468480151</v>
       </c>
       <c r="M12">
         <v>0.8210743283712032</v>
       </c>
       <c r="N12">
-        <v>1.050417126451202</v>
+        <v>1.0504171264512021</v>
       </c>
       <c r="O12">
-        <v>0.9366895607296015</v>
+        <v>0.93668956072960152</v>
       </c>
       <c r="P12">
-        <v>0.9653648472320007</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
+        <v>0.96536484723200067</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1066,49 +1118,49 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>0.9997038147374451</v>
+        <v>0.99970381473744507</v>
       </c>
       <c r="D13">
-        <v>0.9980247514947541</v>
+        <v>0.99802475149475411</v>
       </c>
       <c r="E13">
-        <v>0.9926347079694809</v>
+        <v>0.99263470796948094</v>
       </c>
       <c r="F13">
-        <v>0.9945674475853318</v>
+        <v>0.99456744758533178</v>
       </c>
       <c r="G13">
-        <v>0.9997038147374451</v>
+        <v>0.99970381473744507</v>
       </c>
       <c r="H13">
-        <v>0.9980247514947541</v>
+        <v>0.99802475149475411</v>
       </c>
       <c r="I13">
         <v>0.9945417256556337</v>
       </c>
       <c r="J13">
-        <v>0.9951981430911249</v>
+        <v>0.99519814309112486</v>
       </c>
       <c r="K13">
-        <v>0.9960335587309795</v>
+        <v>0.99603355873097954</v>
       </c>
       <c r="L13">
-        <v>0.994183029362718</v>
+        <v>0.99418302936271796</v>
       </c>
       <c r="M13">
-        <v>0.9996676384160765</v>
+        <v>0.99966763841607653</v>
       </c>
       <c r="N13">
-        <v>0.9953297297321175</v>
+        <v>0.99532972973211753</v>
       </c>
       <c r="O13">
-        <v>0.9962326804467531</v>
+        <v>0.99623268044675306</v>
       </c>
       <c r="P13">
-        <v>0.9956108973284334</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
+        <v>0.99561089732843344</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1116,49 +1168,49 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>0.9357686409085104</v>
+        <v>0.93576864090851042</v>
       </c>
       <c r="D14">
-        <v>0.9768712914227272</v>
+        <v>0.97687129142272722</v>
       </c>
       <c r="E14">
         <v>1.024392138926677</v>
       </c>
       <c r="F14">
-        <v>1.004445348355196</v>
+        <v>1.0044453483551961</v>
       </c>
       <c r="G14">
-        <v>0.9357686409085104</v>
+        <v>0.93576864090851042</v>
       </c>
       <c r="H14">
-        <v>0.9768712914227272</v>
+        <v>0.97687129142272722</v>
       </c>
       <c r="I14">
-        <v>1.000406596344744</v>
+        <v>1.0004065963447439</v>
       </c>
       <c r="J14">
         <v>1.019365122437331</v>
       </c>
       <c r="K14">
-        <v>0.984337981661255</v>
+        <v>0.98433798166125497</v>
       </c>
       <c r="L14">
-        <v>0.9959729712081115</v>
+        <v>0.99597297120811146</v>
       </c>
       <c r="M14">
-        <v>0.9357686409085104</v>
+        <v>0.93576864090851042</v>
       </c>
       <c r="N14">
         <v>1.000631715174702</v>
       </c>
       <c r="O14">
-        <v>0.9853693549032776</v>
+        <v>0.98536935490327759</v>
       </c>
       <c r="P14">
-        <v>0.9926950114080689</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
+        <v>0.99269501140806893</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1166,43 +1218,43 @@
         <v>13</v>
       </c>
       <c r="C15">
-        <v>0.9707473758416045</v>
+        <v>0.97074737584160453</v>
       </c>
       <c r="D15">
         <v>1.072239489946939</v>
       </c>
       <c r="E15">
-        <v>0.9850136336673717</v>
+        <v>0.98501363366737171</v>
       </c>
       <c r="F15">
         <v>1.002521268804754</v>
       </c>
       <c r="G15">
-        <v>0.9707473758416045</v>
+        <v>0.97074737584160453</v>
       </c>
       <c r="H15">
         <v>1.072239489946939</v>
       </c>
       <c r="I15">
-        <v>0.9723512690807741</v>
+        <v>0.97235126908077407</v>
       </c>
       <c r="J15">
-        <v>0.998872779636711</v>
+        <v>0.99887277963671095</v>
       </c>
       <c r="K15">
-        <v>0.9788047132915261</v>
+        <v>0.97880471329152607</v>
       </c>
       <c r="L15">
         <v>1.036646142126203</v>
       </c>
       <c r="M15">
-        <v>0.9707473758416045</v>
+        <v>0.97074737584160453</v>
       </c>
       <c r="N15">
-        <v>1.028626561807155</v>
+        <v>1.0286265618071551</v>
       </c>
       <c r="O15">
-        <v>1.007630442065167</v>
+        <v>1.0076304420651669</v>
       </c>
       <c r="P15">
         <v>1.002149584049485</v>

</xml_diff>